<commit_message>
Added some known errors to the test data sheets to give the QA/QC part something to train against
</commit_message>
<xml_diff>
--- a/Test Data/Nick HV Fake Data.xlsx
+++ b/Test Data/Nick HV Fake Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nick.lyon/Documents/Jobs/2021_HerbVar Network Admin/HerbVar-Data-Portal/Test Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F7D29E4-3EAE-2042-813E-338D30B9DEB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{212DC641-EB50-3745-A601-DB289CE6DFF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-51160" yWindow="2780" windowWidth="28800" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-51160" yWindow="2780" windowWidth="28800" windowHeight="21140" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="siteData" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1187" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1184" uniqueCount="279">
   <si>
     <t>variable</t>
   </si>
@@ -506,13 +506,7 @@
     <t>hemipteraHerbivore</t>
   </si>
   <si>
-    <t>Especially any deviations from protocols and rationale for change(s)</t>
-  </si>
-  <si>
     <t>globalNotes</t>
-  </si>
-  <si>
-    <t>This is the place for any notes that apply to the entire survey/data file</t>
   </si>
   <si>
     <t>percLf15</t>
@@ -1296,9 +1290,6 @@
   </si>
   <si>
     <t>Wanted to try out adding columns to the siteData tab</t>
-  </si>
-  <si>
-    <t>I don't have any notes but I want to demo adding something to every tab</t>
   </si>
 </sst>
 </file>
@@ -2169,7 +2160,7 @@
   </sheetPr>
   <dimension ref="A1:BZ23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A20" sqref="A20:B20"/>
     </sheetView>
@@ -2276,11 +2267,11 @@
         <v>90</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="3" spans="1:78" ht="13" x14ac:dyDescent="0.15">
@@ -2288,11 +2279,11 @@
         <v>91</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="4" spans="1:78" ht="13" x14ac:dyDescent="0.15">
@@ -2300,7 +2291,7 @@
         <v>92</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="3"/>
@@ -2316,7 +2307,7 @@
         <v>4</v>
       </c>
       <c r="D5" s="55" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="6" spans="1:78" ht="13" x14ac:dyDescent="0.15">
@@ -2330,7 +2321,7 @@
         <v>4</v>
       </c>
       <c r="D6" s="55" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="7" spans="1:78" ht="13" x14ac:dyDescent="0.15">
@@ -2398,13 +2389,13 @@
         <v>88</v>
       </c>
       <c r="B11" s="123" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C11" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>237</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>239</v>
       </c>
       <c r="E11" s="122"/>
     </row>
@@ -2413,7 +2404,7 @@
         <v>89</v>
       </c>
       <c r="B12" s="56" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="3" t="s">
@@ -2426,7 +2417,7 @@
         <v>99</v>
       </c>
       <c r="B13" s="123" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="4" t="s">
@@ -2446,7 +2437,7 @@
         <v>5</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="E14" s="122"/>
     </row>
@@ -2455,7 +2446,7 @@
         <v>102</v>
       </c>
       <c r="B15" s="123" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>11</v>
@@ -2470,7 +2461,7 @@
         <v>103</v>
       </c>
       <c r="B16" s="123" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>11</v>
@@ -2485,7 +2476,7 @@
         <v>107</v>
       </c>
       <c r="B17" s="123" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>14</v>
@@ -2500,7 +2491,7 @@
         <v>104</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C18" s="8"/>
       <c r="D18" s="7" t="s">
@@ -2513,7 +2504,7 @@
         <v>105</v>
       </c>
       <c r="B19" s="123" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>17</v>
@@ -2525,14 +2516,14 @@
     </row>
     <row r="20" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A20" s="123" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B20" s="123" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="56" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E20" s="122"/>
     </row>
@@ -2560,7 +2551,7 @@
         <v>119</v>
       </c>
       <c r="D23" s="35" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
   </sheetData>
@@ -2618,7 +2609,7 @@
         <v>84</v>
       </c>
       <c r="D2" s="76" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="85" customFormat="1" ht="14" x14ac:dyDescent="0.15">
@@ -2632,7 +2623,7 @@
         <v>84</v>
       </c>
       <c r="D3" s="84" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -2646,7 +2637,7 @@
         <v>84</v>
       </c>
       <c r="D4" s="76" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="85" customFormat="1" ht="14" x14ac:dyDescent="0.15">
@@ -2660,7 +2651,7 @@
         <v>4</v>
       </c>
       <c r="D5" s="84" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="28" x14ac:dyDescent="0.15">
@@ -2674,7 +2665,7 @@
         <v>4</v>
       </c>
       <c r="D6" s="76" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="85" customFormat="1" ht="14" x14ac:dyDescent="0.15">
@@ -2741,10 +2732,10 @@
         <v>88</v>
       </c>
       <c r="C11" s="84" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D11" s="84" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="14" x14ac:dyDescent="0.15">
@@ -2885,7 +2876,7 @@
     </row>
     <row r="21" spans="1:46" ht="28" x14ac:dyDescent="0.15">
       <c r="A21" s="81" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B21" s="59" t="s">
         <v>111</v>
@@ -2894,12 +2885,12 @@
         <v>78</v>
       </c>
       <c r="D21" s="99" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="22" spans="1:46" s="85" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A22" s="83" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B22" s="53" t="s">
         <v>110</v>
@@ -2908,44 +2899,44 @@
         <v>78</v>
       </c>
       <c r="D22" s="100" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="23" spans="1:46" ht="14" x14ac:dyDescent="0.15">
       <c r="A23" s="81" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B23" s="73" t="s">
         <v>60</v>
       </c>
       <c r="C23" s="99" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D23" s="99" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="24" spans="1:46" s="85" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A24" s="83" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B24" s="52" t="s">
         <v>101</v>
       </c>
       <c r="C24" s="101"/>
       <c r="D24" s="100" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="25" spans="1:46" ht="28" x14ac:dyDescent="0.15">
       <c r="A25" s="81" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B25" s="73" t="s">
         <v>3</v>
       </c>
       <c r="D25" s="76" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="26" spans="1:46" s="98" customFormat="1" ht="13" x14ac:dyDescent="0.15">
@@ -2965,7 +2956,7 @@
         <v>64</v>
       </c>
       <c r="D27" s="99" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="28" spans="1:46" s="85" customFormat="1" ht="28" x14ac:dyDescent="0.15">
@@ -2979,7 +2970,7 @@
         <v>62</v>
       </c>
       <c r="D28" s="84" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="29" spans="1:46" ht="28" x14ac:dyDescent="0.15">
@@ -2993,7 +2984,7 @@
         <v>65</v>
       </c>
       <c r="D29" s="99" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="30" spans="1:46" s="85" customFormat="1" ht="28" x14ac:dyDescent="0.15">
@@ -3007,7 +2998,7 @@
         <v>64</v>
       </c>
       <c r="D30" s="100" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="31" spans="1:46" ht="14" x14ac:dyDescent="0.15">
@@ -3120,7 +3111,7 @@
         <v>71</v>
       </c>
       <c r="D37" s="76" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="AO37" s="59"/>
       <c r="AP37" s="59"/>
@@ -3161,7 +3152,7 @@
         <v>76</v>
       </c>
       <c r="D39" s="76" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="AM39" s="59"/>
       <c r="AN39" s="59"/>
@@ -3249,13 +3240,13 @@
         <v>63</v>
       </c>
       <c r="B43" s="58" t="s">
+        <v>240</v>
+      </c>
+      <c r="C43" s="107" t="s">
+        <v>241</v>
+      </c>
+      <c r="D43" s="99" t="s">
         <v>242</v>
-      </c>
-      <c r="C43" s="107" t="s">
-        <v>243</v>
-      </c>
-      <c r="D43" s="99" t="s">
-        <v>244</v>
       </c>
       <c r="AI43" s="59"/>
       <c r="AJ43" s="59"/>
@@ -3308,7 +3299,7 @@
         <v>68</v>
       </c>
       <c r="D45" s="76" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="AG45" s="59"/>
       <c r="AH45" s="59"/>
@@ -3336,7 +3327,7 @@
         <v>72</v>
       </c>
       <c r="D46" s="100" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="AF46" s="53"/>
       <c r="AG46" s="53"/>
@@ -3361,10 +3352,10 @@
         <v>132</v>
       </c>
       <c r="C47" s="99" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D47" s="99" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="AE47" s="59"/>
       <c r="AF47" s="59"/>
@@ -3391,10 +3382,10 @@
         <v>133</v>
       </c>
       <c r="C48" s="108" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D48" s="100" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="AD48" s="60"/>
       <c r="AE48" s="53"/>
@@ -3419,13 +3410,13 @@
         <v>63</v>
       </c>
       <c r="B49" s="58" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C49" s="75" t="s">
         <v>68</v>
       </c>
       <c r="D49" s="76" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="U49" s="57"/>
       <c r="V49" s="57"/>
@@ -3457,7 +3448,7 @@
         <v>84</v>
       </c>
       <c r="D50" s="84" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E50" s="61"/>
       <c r="F50" s="60"/>
@@ -3507,13 +3498,13 @@
         <v>63</v>
       </c>
       <c r="B51" s="59" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C51" s="75" t="s">
         <v>68</v>
       </c>
       <c r="D51" s="76" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E51" s="59"/>
       <c r="F51" s="59"/>
@@ -3608,7 +3599,7 @@
     </row>
     <row r="53" spans="1:46" ht="28" x14ac:dyDescent="0.15">
       <c r="A53" s="81" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B53" s="109" t="s">
         <v>18</v>
@@ -3617,12 +3608,12 @@
         <v>64</v>
       </c>
       <c r="D53" s="99" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="54" spans="1:46" s="85" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A54" s="83" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B54" s="64" t="s">
         <v>90</v>
@@ -3631,12 +3622,12 @@
         <v>64</v>
       </c>
       <c r="D54" s="84" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="55" spans="1:46" ht="28" x14ac:dyDescent="0.15">
       <c r="A55" s="81" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B55" s="109" t="s">
         <v>11</v>
@@ -3645,12 +3636,12 @@
         <v>65</v>
       </c>
       <c r="D55" s="99" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="56" spans="1:46" s="85" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A56" s="83" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B56" s="64" t="s">
         <v>19</v>
@@ -3659,12 +3650,12 @@
         <v>64</v>
       </c>
       <c r="D56" s="100" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="57" spans="1:46" ht="28" x14ac:dyDescent="0.15">
       <c r="A57" s="81" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B57" s="109" t="s">
         <v>20</v>
@@ -3673,12 +3664,12 @@
         <v>72</v>
       </c>
       <c r="D57" s="76" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="58" spans="1:46" s="85" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A58" s="83" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B58" s="110" t="s">
         <v>44</v>
@@ -3692,35 +3683,35 @@
     </row>
     <row r="59" spans="1:46" ht="28" x14ac:dyDescent="0.15">
       <c r="A59" s="81" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B59" s="111" t="s">
         <v>120</v>
       </c>
       <c r="C59" s="76" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D59" s="107" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="60" spans="1:46" s="85" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A60" s="83" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B60" s="110" t="s">
         <v>121</v>
       </c>
       <c r="C60" s="100" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D60" s="100" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="61" spans="1:46" ht="28" x14ac:dyDescent="0.15">
       <c r="A61" s="81" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B61" s="111" t="s">
         <v>45</v>
@@ -3734,7 +3725,7 @@
     </row>
     <row r="62" spans="1:46" s="85" customFormat="1" ht="70" x14ac:dyDescent="0.15">
       <c r="A62" s="83" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B62" s="110" t="s">
         <v>46</v>
@@ -3743,12 +3734,12 @@
         <v>71</v>
       </c>
       <c r="D62" s="84" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="63" spans="1:46" ht="14" x14ac:dyDescent="0.15">
       <c r="A63" s="81" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B63" s="109" t="s">
         <v>127</v>
@@ -3757,12 +3748,12 @@
         <v>71</v>
       </c>
       <c r="D63" s="99" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="64" spans="1:46" s="85" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A64" s="83" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B64" s="64" t="s">
         <v>128</v>
@@ -3771,12 +3762,12 @@
         <v>71</v>
       </c>
       <c r="D64" s="100" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="65" spans="1:19" ht="28" x14ac:dyDescent="0.15">
       <c r="A65" s="81" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B65" s="109" t="s">
         <v>129</v>
@@ -3785,12 +3776,12 @@
         <v>71</v>
       </c>
       <c r="D65" s="99" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="66" spans="1:19" s="85" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A66" s="83" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B66" s="64" t="s">
         <v>130</v>
@@ -3799,12 +3790,12 @@
         <v>71</v>
       </c>
       <c r="D66" s="100" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="67" spans="1:19" ht="70" x14ac:dyDescent="0.15">
       <c r="A67" s="81" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B67" s="111" t="s">
         <v>47</v>
@@ -3813,12 +3804,12 @@
         <v>68</v>
       </c>
       <c r="D67" s="76" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="68" spans="1:19" s="85" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A68" s="83" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B68" s="64" t="s">
         <v>138</v>
@@ -3827,12 +3818,12 @@
         <v>68</v>
       </c>
       <c r="D68" s="100" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="69" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A69" s="81" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B69" s="109" t="s">
         <v>139</v>
@@ -3841,12 +3832,12 @@
         <v>68</v>
       </c>
       <c r="D69" s="99" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="70" spans="1:19" s="85" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A70" s="83" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B70" s="64" t="s">
         <v>140</v>
@@ -3855,12 +3846,12 @@
         <v>68</v>
       </c>
       <c r="D70" s="100" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="71" spans="1:19" ht="28" x14ac:dyDescent="0.15">
       <c r="A71" s="81" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B71" s="109" t="s">
         <v>141</v>
@@ -3869,26 +3860,26 @@
         <v>68</v>
       </c>
       <c r="D71" s="99" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="72" spans="1:19" s="85" customFormat="1" ht="56" x14ac:dyDescent="0.15">
       <c r="A72" s="83" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B72" s="110" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C72" s="108" t="s">
         <v>68</v>
       </c>
       <c r="D72" s="84" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="73" spans="1:19" ht="28" x14ac:dyDescent="0.15">
       <c r="A73" s="81" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B73" s="109" t="s">
         <v>3</v>
@@ -3897,7 +3888,7 @@
         <v>84</v>
       </c>
       <c r="D73" s="76" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="74" spans="1:19" s="98" customFormat="1" ht="13" x14ac:dyDescent="0.15">
@@ -3908,7 +3899,7 @@
     </row>
     <row r="75" spans="1:19" ht="28" x14ac:dyDescent="0.15">
       <c r="A75" s="81" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B75" s="58" t="s">
         <v>18</v>
@@ -3917,12 +3908,12 @@
         <v>64</v>
       </c>
       <c r="D75" s="99" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="76" spans="1:19" s="85" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A76" s="83" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B76" s="61" t="s">
         <v>90</v>
@@ -3931,12 +3922,12 @@
         <v>64</v>
       </c>
       <c r="D76" s="84" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="77" spans="1:19" ht="28" x14ac:dyDescent="0.15">
       <c r="A77" s="81" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B77" s="58" t="s">
         <v>11</v>
@@ -3945,12 +3936,12 @@
         <v>65</v>
       </c>
       <c r="D77" s="99" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="78" spans="1:19" s="85" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A78" s="83" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B78" s="61" t="s">
         <v>19</v>
@@ -3959,14 +3950,14 @@
         <v>64</v>
       </c>
       <c r="D78" s="100" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="R78" s="61"/>
       <c r="S78" s="60"/>
     </row>
     <row r="79" spans="1:19" ht="28" x14ac:dyDescent="0.15">
       <c r="A79" s="81" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B79" s="58" t="s">
         <v>20</v>
@@ -3975,7 +3966,7 @@
         <v>72</v>
       </c>
       <c r="D79" s="76" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="Q79" s="58"/>
       <c r="R79" s="58"/>
@@ -3983,7 +3974,7 @@
     </row>
     <row r="80" spans="1:19" s="85" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A80" s="83" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B80" s="61" t="s">
         <v>134</v>
@@ -3992,7 +3983,7 @@
         <v>71</v>
       </c>
       <c r="D80" s="84" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="P80" s="61"/>
       <c r="Q80" s="61"/>
@@ -4001,7 +3992,7 @@
     </row>
     <row r="81" spans="1:28" ht="28" x14ac:dyDescent="0.15">
       <c r="A81" s="81" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B81" s="58" t="s">
         <v>135</v>
@@ -4010,7 +4001,7 @@
         <v>71</v>
       </c>
       <c r="D81" s="76" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="O81" s="58"/>
       <c r="P81" s="58"/>
@@ -4020,16 +4011,16 @@
     </row>
     <row r="82" spans="1:28" s="85" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A82" s="83" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B82" s="61" t="s">
         <v>144</v>
       </c>
       <c r="C82" s="116" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D82" s="117" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="N82" s="61"/>
       <c r="O82" s="61"/>
@@ -4040,7 +4031,7 @@
     </row>
     <row r="83" spans="1:28" ht="28" x14ac:dyDescent="0.15">
       <c r="A83" s="81" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B83" s="58" t="s">
         <v>41</v>
@@ -4049,7 +4040,7 @@
         <v>71</v>
       </c>
       <c r="D83" s="76" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="M83" s="58"/>
       <c r="N83" s="58"/>
@@ -4061,7 +4052,7 @@
     </row>
     <row r="84" spans="1:28" s="85" customFormat="1" ht="42" x14ac:dyDescent="0.15">
       <c r="A84" s="83" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B84" s="61" t="s">
         <v>136</v>
@@ -4070,7 +4061,7 @@
         <v>71</v>
       </c>
       <c r="D84" s="84" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="L84" s="60"/>
       <c r="M84" s="61"/>
@@ -4083,7 +4074,7 @@
     </row>
     <row r="85" spans="1:28" ht="28" x14ac:dyDescent="0.15">
       <c r="A85" s="81" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B85" s="58" t="s">
         <v>42</v>
@@ -4092,7 +4083,7 @@
         <v>71</v>
       </c>
       <c r="D85" s="76" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="K85" s="57"/>
       <c r="L85" s="57"/>
@@ -4106,7 +4097,7 @@
     </row>
     <row r="86" spans="1:28" s="85" customFormat="1" ht="56" x14ac:dyDescent="0.15">
       <c r="A86" s="83" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B86" s="61" t="s">
         <v>43</v>
@@ -4115,12 +4106,12 @@
         <v>71</v>
       </c>
       <c r="D86" s="84" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="87" spans="1:28" ht="56" x14ac:dyDescent="0.15">
       <c r="A87" s="81" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B87" s="58" t="s">
         <v>143</v>
@@ -4129,12 +4120,12 @@
         <v>71</v>
       </c>
       <c r="D87" s="76" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="88" spans="1:28" s="85" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A88" s="83" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B88" s="61" t="s">
         <v>137</v>
@@ -4143,26 +4134,26 @@
         <v>71</v>
       </c>
       <c r="D88" s="100" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="89" spans="1:28" ht="28" x14ac:dyDescent="0.15">
       <c r="A89" s="81" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B89" s="58" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C89" s="87" t="s">
         <v>71</v>
       </c>
       <c r="D89" s="99" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="90" spans="1:28" s="85" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A90" s="83" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B90" s="61" t="s">
         <v>145</v>
@@ -4171,7 +4162,7 @@
         <v>71</v>
       </c>
       <c r="D90" s="100" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="F90" s="62"/>
       <c r="G90" s="62"/>
@@ -4197,9 +4188,9 @@
       <c r="AA90" s="62"/>
       <c r="AB90" s="62"/>
     </row>
-    <row r="91" spans="1:28" ht="28" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:28" ht="14" x14ac:dyDescent="0.15">
       <c r="A91" s="81" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B91" s="58" t="s">
         <v>146</v>
@@ -4208,7 +4199,7 @@
         <v>71</v>
       </c>
       <c r="D91" s="99" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E91" s="118"/>
       <c r="F91" s="118"/>
@@ -4237,7 +4228,7 @@
     </row>
     <row r="92" spans="1:28" s="85" customFormat="1" ht="56" x14ac:dyDescent="0.15">
       <c r="A92" s="83" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B92" s="61" t="s">
         <v>147</v>
@@ -4246,7 +4237,7 @@
         <v>71</v>
       </c>
       <c r="D92" s="100" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="E92" s="62"/>
       <c r="F92" s="62"/>
@@ -4275,7 +4266,7 @@
     </row>
     <row r="93" spans="1:28" ht="28" x14ac:dyDescent="0.15">
       <c r="A93" s="81" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B93" s="58" t="s">
         <v>3</v>
@@ -4284,7 +4275,7 @@
         <v>84</v>
       </c>
       <c r="D93" s="76" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E93" s="118"/>
       <c r="F93" s="118"/>
@@ -4322,10 +4313,10 @@
         <v>3</v>
       </c>
       <c r="B95" s="59" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D95" s="99" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="99" ht="13" x14ac:dyDescent="0.15"/>
@@ -4446,7 +4437,7 @@
         <v>30</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="13" x14ac:dyDescent="0.15">
@@ -4596,7 +4587,7 @@
         <v>28</v>
       </c>
       <c r="Q1" s="61" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="R1" s="60" t="s">
         <v>29</v>
@@ -4647,64 +4638,64 @@
         <v>3</v>
       </c>
       <c r="AH1" s="61" t="s">
+        <v>169</v>
+      </c>
+      <c r="AI1" s="61" t="s">
+        <v>170</v>
+      </c>
+      <c r="AJ1" s="61" t="s">
         <v>171</v>
       </c>
-      <c r="AI1" s="61" t="s">
+      <c r="AK1" s="61" t="s">
         <v>172</v>
       </c>
-      <c r="AJ1" s="61" t="s">
-        <v>173</v>
-      </c>
-      <c r="AK1" s="61" t="s">
-        <v>174</v>
-      </c>
       <c r="AL1" s="53" t="s">
+        <v>149</v>
+      </c>
+      <c r="AM1" s="53" t="s">
+        <v>150</v>
+      </c>
+      <c r="AN1" s="53" t="s">
         <v>151</v>
       </c>
-      <c r="AM1" s="53" t="s">
+      <c r="AO1" s="53" t="s">
         <v>152</v>
       </c>
-      <c r="AN1" s="53" t="s">
+      <c r="AP1" s="53" t="s">
         <v>153</v>
       </c>
-      <c r="AO1" s="53" t="s">
+      <c r="AQ1" s="53" t="s">
         <v>154</v>
       </c>
-      <c r="AP1" s="53" t="s">
+      <c r="AR1" s="53" t="s">
         <v>155</v>
       </c>
-      <c r="AQ1" s="53" t="s">
+      <c r="AS1" s="53" t="s">
         <v>156</v>
       </c>
-      <c r="AR1" s="53" t="s">
+      <c r="AT1" s="53" t="s">
         <v>157</v>
       </c>
-      <c r="AS1" s="53" t="s">
+      <c r="AU1" s="53" t="s">
         <v>158</v>
       </c>
-      <c r="AT1" s="53" t="s">
+      <c r="AV1" s="53" t="s">
         <v>159</v>
       </c>
-      <c r="AU1" s="53" t="s">
+      <c r="AW1" s="53" t="s">
         <v>160</v>
       </c>
-      <c r="AV1" s="53" t="s">
+      <c r="AX1" s="53" t="s">
         <v>161</v>
       </c>
-      <c r="AW1" s="53" t="s">
+      <c r="AY1" s="53" t="s">
         <v>162</v>
       </c>
-      <c r="AX1" s="53" t="s">
+      <c r="AZ1" s="53" t="s">
         <v>163</v>
       </c>
-      <c r="AY1" s="53" t="s">
+      <c r="BA1" s="53" t="s">
         <v>164</v>
-      </c>
-      <c r="AZ1" s="53" t="s">
-        <v>165</v>
-      </c>
-      <c r="BA1" s="53" t="s">
-        <v>166</v>
       </c>
       <c r="BB1" s="30"/>
       <c r="BC1" s="29"/>
@@ -4718,16 +4709,16 @@
     </row>
     <row r="2" spans="1:62" ht="16" x14ac:dyDescent="0.15">
       <c r="A2" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B2" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C2" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D2" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B2" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C2" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D2" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E2" s="37">
         <v>1</v>
@@ -4773,16 +4764,16 @@
     </row>
     <row r="3" spans="1:62" ht="16" x14ac:dyDescent="0.15">
       <c r="A3" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B3" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C3" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D3" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B3" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C3" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D3" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E3" s="37">
         <v>1</v>
@@ -4791,7 +4782,7 @@
         <v>1</v>
       </c>
       <c r="G3" s="124" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="H3" s="38"/>
       <c r="I3" s="37"/>
@@ -4827,16 +4818,16 @@
     </row>
     <row r="4" spans="1:62" ht="16" x14ac:dyDescent="0.15">
       <c r="A4" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B4" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C4" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D4" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B4" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C4" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D4" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E4" s="37">
         <v>1</v>
@@ -4881,16 +4872,16 @@
     </row>
     <row r="5" spans="1:62" ht="16" x14ac:dyDescent="0.15">
       <c r="A5" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B5" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C5" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D5" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B5" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C5" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D5" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E5" s="37">
         <v>1</v>
@@ -4899,7 +4890,7 @@
         <v>1</v>
       </c>
       <c r="G5" s="124" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="H5" s="37"/>
       <c r="I5" s="37"/>
@@ -4935,16 +4926,16 @@
     </row>
     <row r="6" spans="1:62" ht="16" x14ac:dyDescent="0.15">
       <c r="A6" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B6" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C6" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D6" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B6" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C6" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D6" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E6" s="37">
         <v>1</v>
@@ -4989,16 +4980,16 @@
     </row>
     <row r="7" spans="1:62" ht="16" x14ac:dyDescent="0.15">
       <c r="A7" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B7" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C7" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D7" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B7" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C7" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D7" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E7" s="37">
         <v>2</v>
@@ -5007,7 +4998,7 @@
         <v>2</v>
       </c>
       <c r="G7" s="124" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="H7" s="38"/>
       <c r="I7" s="37"/>
@@ -5043,16 +5034,16 @@
     </row>
     <row r="8" spans="1:62" ht="16" x14ac:dyDescent="0.15">
       <c r="A8" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B8" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C8" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D8" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B8" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C8" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D8" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E8" s="37">
         <v>2</v>
@@ -5097,16 +5088,16 @@
     </row>
     <row r="9" spans="1:62" ht="16" x14ac:dyDescent="0.15">
       <c r="A9" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B9" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C9" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D9" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B9" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C9" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D9" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E9" s="37">
         <v>2</v>
@@ -5115,7 +5106,7 @@
         <v>2</v>
       </c>
       <c r="G9" s="124" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="H9" s="38"/>
       <c r="I9" s="37"/>
@@ -5151,16 +5142,16 @@
     </row>
     <row r="10" spans="1:62" ht="16" x14ac:dyDescent="0.15">
       <c r="A10" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B10" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C10" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D10" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B10" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C10" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D10" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E10" s="37">
         <v>2</v>
@@ -5205,16 +5196,16 @@
     </row>
     <row r="11" spans="1:62" ht="16" x14ac:dyDescent="0.15">
       <c r="A11" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B11" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C11" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D11" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B11" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C11" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D11" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E11" s="37">
         <v>2</v>
@@ -5223,7 +5214,7 @@
         <v>2</v>
       </c>
       <c r="G11" s="124" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="H11" s="38"/>
       <c r="I11" s="37"/>
@@ -5259,16 +5250,16 @@
     </row>
     <row r="12" spans="1:62" ht="16" x14ac:dyDescent="0.15">
       <c r="A12" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B12" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C12" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D12" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B12" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C12" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D12" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E12" s="37">
         <v>6</v>
@@ -5313,16 +5304,16 @@
     </row>
     <row r="13" spans="1:62" ht="16" x14ac:dyDescent="0.15">
       <c r="A13" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B13" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C13" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D13" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B13" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C13" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D13" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E13" s="37">
         <v>6</v>
@@ -5331,7 +5322,7 @@
         <v>6</v>
       </c>
       <c r="G13" s="124" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="H13" s="38"/>
       <c r="I13" s="37"/>
@@ -5367,16 +5358,16 @@
     </row>
     <row r="14" spans="1:62" ht="16" x14ac:dyDescent="0.15">
       <c r="A14" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B14" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C14" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D14" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B14" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C14" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D14" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E14" s="37">
         <v>6</v>
@@ -5421,16 +5412,16 @@
     </row>
     <row r="15" spans="1:62" ht="16" x14ac:dyDescent="0.15">
       <c r="A15" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B15" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C15" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D15" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B15" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C15" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D15" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E15" s="37">
         <v>6</v>
@@ -5439,7 +5430,7 @@
         <v>6</v>
       </c>
       <c r="G15" s="124" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="H15" s="38"/>
       <c r="I15" s="37"/>
@@ -5475,16 +5466,16 @@
     </row>
     <row r="16" spans="1:62" ht="16" x14ac:dyDescent="0.15">
       <c r="A16" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B16" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C16" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D16" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B16" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C16" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D16" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E16" s="37">
         <v>6</v>
@@ -5527,16 +5518,16 @@
     </row>
     <row r="17" spans="1:37" ht="16" x14ac:dyDescent="0.15">
       <c r="A17" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B17" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C17" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D17" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B17" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C17" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D17" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E17" s="37">
         <v>6</v>
@@ -5579,16 +5570,16 @@
     </row>
     <row r="18" spans="1:37" ht="16" x14ac:dyDescent="0.15">
       <c r="A18" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B18" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C18" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D18" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B18" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C18" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D18" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E18" s="37">
         <v>6</v>
@@ -5631,16 +5622,16 @@
     </row>
     <row r="19" spans="1:37" ht="16" x14ac:dyDescent="0.15">
       <c r="A19" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B19" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C19" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D19" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B19" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C19" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D19" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E19" s="37">
         <v>32</v>
@@ -5683,16 +5674,16 @@
     </row>
     <row r="20" spans="1:37" ht="16" x14ac:dyDescent="0.15">
       <c r="A20" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B20" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C20" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D20" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B20" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C20" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D20" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E20" s="37">
         <v>32</v>
@@ -5735,16 +5726,16 @@
     </row>
     <row r="21" spans="1:37" ht="16" x14ac:dyDescent="0.15">
       <c r="A21" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B21" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C21" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D21" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B21" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C21" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D21" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E21" s="37">
         <v>32</v>
@@ -5787,16 +5778,16 @@
     </row>
     <row r="22" spans="1:37" ht="16" x14ac:dyDescent="0.15">
       <c r="A22" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B22" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C22" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D22" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B22" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C22" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D22" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E22" s="37">
         <v>32</v>
@@ -5839,16 +5830,16 @@
     </row>
     <row r="23" spans="1:37" ht="16" x14ac:dyDescent="0.15">
       <c r="A23" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B23" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C23" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D23" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B23" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C23" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D23" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E23" s="37">
         <v>32</v>
@@ -5891,16 +5882,16 @@
     </row>
     <row r="24" spans="1:37" ht="16" x14ac:dyDescent="0.15">
       <c r="A24" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B24" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C24" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D24" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B24" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C24" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D24" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E24" s="37">
         <v>32</v>
@@ -5943,16 +5934,16 @@
     </row>
     <row r="25" spans="1:37" ht="16" x14ac:dyDescent="0.15">
       <c r="A25" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B25" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C25" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D25" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B25" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C25" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D25" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E25" s="37">
         <v>32</v>
@@ -5995,16 +5986,16 @@
     </row>
     <row r="26" spans="1:37" ht="16" x14ac:dyDescent="0.15">
       <c r="A26" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B26" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C26" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D26" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B26" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C26" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D26" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E26" s="37">
         <v>32</v>
@@ -6047,16 +6038,16 @@
     </row>
     <row r="27" spans="1:37" ht="16" x14ac:dyDescent="0.15">
       <c r="A27" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B27" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C27" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D27" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B27" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C27" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D27" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E27" s="37">
         <v>32</v>
@@ -6099,22 +6090,22 @@
     </row>
     <row r="28" spans="1:37" ht="16" x14ac:dyDescent="0.15">
       <c r="A28" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B28" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C28" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D28" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B28" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C28" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D28" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E28" s="37">
         <v>86</v>
       </c>
       <c r="F28" s="124" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="G28" s="26"/>
       <c r="H28" s="38"/>
@@ -6151,16 +6142,16 @@
     </row>
     <row r="29" spans="1:37" ht="16" x14ac:dyDescent="0.15">
       <c r="A29" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B29" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C29" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D29" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B29" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C29" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D29" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E29" s="37">
         <v>86</v>
@@ -6203,16 +6194,16 @@
     </row>
     <row r="30" spans="1:37" ht="16" x14ac:dyDescent="0.15">
       <c r="A30" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B30" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C30" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D30" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B30" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C30" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D30" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E30" s="37">
         <v>86</v>
@@ -6255,16 +6246,16 @@
     </row>
     <row r="31" spans="1:37" ht="16" x14ac:dyDescent="0.15">
       <c r="A31" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B31" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C31" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D31" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B31" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C31" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D31" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E31" s="37">
         <v>86</v>
@@ -6307,16 +6298,16 @@
     </row>
     <row r="32" spans="1:37" ht="13" x14ac:dyDescent="0.15">
       <c r="A32" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B32" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C32" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D32" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B32" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C32" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D32" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E32" s="37">
         <v>86</v>
@@ -6359,16 +6350,16 @@
     </row>
     <row r="33" spans="1:37" ht="13" x14ac:dyDescent="0.15">
       <c r="A33" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B33" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C33" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D33" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B33" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C33" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D33" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E33" s="37">
         <v>86</v>
@@ -6411,16 +6402,16 @@
     </row>
     <row r="34" spans="1:37" ht="13" x14ac:dyDescent="0.15">
       <c r="A34" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B34" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C34" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D34" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B34" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C34" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D34" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E34" s="37">
         <v>86</v>
@@ -6463,16 +6454,16 @@
     </row>
     <row r="35" spans="1:37" ht="13" x14ac:dyDescent="0.15">
       <c r="A35" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B35" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C35" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D35" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B35" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C35" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D35" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E35" s="37">
         <v>68</v>
@@ -6515,16 +6506,16 @@
     </row>
     <row r="36" spans="1:37" ht="13" x14ac:dyDescent="0.15">
       <c r="A36" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B36" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C36" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D36" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B36" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C36" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D36" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E36" s="37">
         <v>68</v>
@@ -6567,16 +6558,16 @@
     </row>
     <row r="37" spans="1:37" ht="13" x14ac:dyDescent="0.15">
       <c r="A37" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B37" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C37" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D37" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B37" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C37" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D37" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E37" s="37">
         <v>86</v>
@@ -6619,16 +6610,16 @@
     </row>
     <row r="38" spans="1:37" ht="13" x14ac:dyDescent="0.15">
       <c r="A38" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B38" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C38" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D38" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B38" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C38" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D38" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E38" s="37">
         <v>86</v>
@@ -6671,16 +6662,16 @@
     </row>
     <row r="39" spans="1:37" ht="13" x14ac:dyDescent="0.15">
       <c r="A39" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B39" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C39" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D39" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B39" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C39" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D39" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E39" s="37"/>
       <c r="F39" s="37"/>
@@ -6719,16 +6710,16 @@
     </row>
     <row r="40" spans="1:37" ht="13" x14ac:dyDescent="0.15">
       <c r="A40" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B40" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C40" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D40" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B40" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C40" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D40" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E40" s="37"/>
       <c r="F40" s="37"/>
@@ -6767,16 +6758,16 @@
     </row>
     <row r="41" spans="1:37" ht="13" x14ac:dyDescent="0.15">
       <c r="A41" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B41" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C41" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D41" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B41" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C41" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D41" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E41" s="37"/>
       <c r="F41" s="37"/>
@@ -6815,16 +6806,16 @@
     </row>
     <row r="42" spans="1:37" ht="13" x14ac:dyDescent="0.15">
       <c r="A42" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B42" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C42" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D42" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B42" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C42" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D42" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E42" s="37"/>
       <c r="F42" s="37"/>
@@ -6863,16 +6854,16 @@
     </row>
     <row r="43" spans="1:37" ht="13" x14ac:dyDescent="0.15">
       <c r="A43" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B43" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C43" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D43" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B43" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C43" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D43" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E43" s="37"/>
       <c r="F43" s="37"/>
@@ -6911,16 +6902,16 @@
     </row>
     <row r="44" spans="1:37" ht="13" x14ac:dyDescent="0.15">
       <c r="A44" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B44" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C44" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D44" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B44" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C44" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D44" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E44" s="37"/>
       <c r="F44" s="37"/>
@@ -6959,16 +6950,16 @@
     </row>
     <row r="45" spans="1:37" ht="13" x14ac:dyDescent="0.15">
       <c r="A45" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B45" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C45" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D45" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B45" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C45" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D45" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E45" s="37"/>
       <c r="F45" s="37"/>
@@ -7007,16 +6998,16 @@
     </row>
     <row r="46" spans="1:37" ht="13" x14ac:dyDescent="0.15">
       <c r="A46" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B46" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C46" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D46" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B46" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C46" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D46" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E46" s="37"/>
       <c r="F46" s="37"/>
@@ -7055,16 +7046,16 @@
     </row>
     <row r="47" spans="1:37" ht="13" x14ac:dyDescent="0.15">
       <c r="A47" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B47" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C47" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D47" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B47" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C47" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D47" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E47" s="37"/>
       <c r="F47" s="37"/>
@@ -7103,16 +7094,16 @@
     </row>
     <row r="48" spans="1:37" ht="13" x14ac:dyDescent="0.15">
       <c r="A48" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B48" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C48" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D48" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B48" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C48" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D48" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E48" s="37"/>
       <c r="F48" s="37"/>
@@ -7151,16 +7142,16 @@
     </row>
     <row r="49" spans="1:37" ht="13" x14ac:dyDescent="0.15">
       <c r="A49" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B49" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C49" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D49" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B49" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C49" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D49" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E49" s="37"/>
       <c r="F49" s="37"/>
@@ -7199,16 +7190,16 @@
     </row>
     <row r="50" spans="1:37" ht="13" x14ac:dyDescent="0.15">
       <c r="A50" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B50" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C50" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D50" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B50" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C50" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D50" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E50" s="37"/>
       <c r="F50" s="37"/>
@@ -7247,16 +7238,16 @@
     </row>
     <row r="51" spans="1:37" ht="13" x14ac:dyDescent="0.15">
       <c r="A51" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B51" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C51" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D51" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B51" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C51" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D51" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E51" s="37"/>
       <c r="F51" s="37"/>
@@ -7295,16 +7286,16 @@
     </row>
     <row r="52" spans="1:37" ht="13" x14ac:dyDescent="0.15">
       <c r="A52" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B52" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C52" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D52" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B52" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C52" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D52" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E52" s="37"/>
       <c r="F52" s="37"/>
@@ -7343,16 +7334,16 @@
     </row>
     <row r="53" spans="1:37" ht="13" x14ac:dyDescent="0.15">
       <c r="A53" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B53" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C53" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D53" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B53" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C53" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D53" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E53" s="37"/>
       <c r="F53" s="37"/>
@@ -7391,16 +7382,16 @@
     </row>
     <row r="54" spans="1:37" ht="13" x14ac:dyDescent="0.15">
       <c r="A54" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B54" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C54" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D54" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B54" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C54" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D54" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E54" s="37"/>
       <c r="F54" s="37"/>
@@ -7439,16 +7430,16 @@
     </row>
     <row r="55" spans="1:37" ht="13" x14ac:dyDescent="0.15">
       <c r="A55" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B55" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C55" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D55" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B55" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C55" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D55" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E55" s="37"/>
       <c r="F55" s="37"/>
@@ -7487,16 +7478,16 @@
     </row>
     <row r="56" spans="1:37" ht="13" x14ac:dyDescent="0.15">
       <c r="A56" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B56" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C56" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D56" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B56" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C56" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D56" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E56" s="37"/>
       <c r="F56" s="37"/>
@@ -7535,16 +7526,16 @@
     </row>
     <row r="57" spans="1:37" ht="13" x14ac:dyDescent="0.15">
       <c r="A57" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B57" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C57" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D57" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B57" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C57" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D57" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E57" s="37"/>
       <c r="F57" s="37"/>
@@ -7583,16 +7574,16 @@
     </row>
     <row r="58" spans="1:37" ht="13" x14ac:dyDescent="0.15">
       <c r="A58" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B58" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C58" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D58" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B58" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C58" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D58" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E58" s="37"/>
       <c r="F58" s="37"/>
@@ -7631,16 +7622,16 @@
     </row>
     <row r="59" spans="1:37" ht="13" x14ac:dyDescent="0.15">
       <c r="A59" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B59" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C59" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D59" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B59" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C59" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D59" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E59" s="37"/>
       <c r="F59" s="37"/>
@@ -7679,16 +7670,16 @@
     </row>
     <row r="60" spans="1:37" ht="13" x14ac:dyDescent="0.15">
       <c r="A60" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B60" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C60" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D60" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B60" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C60" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D60" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E60" s="37"/>
       <c r="F60" s="37"/>
@@ -7727,16 +7718,16 @@
     </row>
     <row r="61" spans="1:37" ht="13" x14ac:dyDescent="0.15">
       <c r="A61" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B61" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C61" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D61" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B61" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C61" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D61" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E61" s="37"/>
       <c r="F61" s="37"/>
@@ -7775,16 +7766,16 @@
     </row>
     <row r="62" spans="1:37" ht="13" x14ac:dyDescent="0.15">
       <c r="A62" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B62" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C62" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D62" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B62" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C62" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D62" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E62" s="37"/>
       <c r="F62" s="37"/>
@@ -7823,16 +7814,16 @@
     </row>
     <row r="63" spans="1:37" ht="13" x14ac:dyDescent="0.15">
       <c r="A63" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B63" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C63" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D63" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B63" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C63" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D63" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E63" s="37"/>
       <c r="F63" s="37"/>
@@ -7871,16 +7862,16 @@
     </row>
     <row r="64" spans="1:37" ht="13" x14ac:dyDescent="0.15">
       <c r="A64" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B64" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C64" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D64" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B64" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C64" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D64" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E64" s="37"/>
       <c r="F64" s="37"/>
@@ -7919,16 +7910,16 @@
     </row>
     <row r="65" spans="1:37" ht="13" x14ac:dyDescent="0.15">
       <c r="A65" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B65" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C65" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D65" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B65" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C65" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D65" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E65" s="37"/>
       <c r="F65" s="37"/>
@@ -7967,16 +7958,16 @@
     </row>
     <row r="66" spans="1:37" ht="13" x14ac:dyDescent="0.15">
       <c r="A66" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B66" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C66" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D66" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B66" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C66" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D66" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E66" s="37"/>
       <c r="F66" s="37"/>
@@ -8015,16 +8006,16 @@
     </row>
     <row r="67" spans="1:37" ht="13" x14ac:dyDescent="0.15">
       <c r="A67" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B67" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C67" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D67" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B67" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C67" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D67" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E67" s="37"/>
       <c r="F67" s="37"/>
@@ -8063,16 +8054,16 @@
     </row>
     <row r="68" spans="1:37" ht="13" x14ac:dyDescent="0.15">
       <c r="A68" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B68" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C68" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D68" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B68" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C68" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D68" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E68" s="37"/>
       <c r="F68" s="37"/>
@@ -8111,16 +8102,16 @@
     </row>
     <row r="69" spans="1:37" ht="13" x14ac:dyDescent="0.15">
       <c r="A69" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B69" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C69" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D69" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B69" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C69" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D69" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E69" s="37"/>
       <c r="F69" s="37"/>
@@ -8159,16 +8150,16 @@
     </row>
     <row r="70" spans="1:37" ht="13" x14ac:dyDescent="0.15">
       <c r="A70" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B70" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C70" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D70" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B70" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C70" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D70" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E70" s="37"/>
       <c r="F70" s="37"/>
@@ -8207,16 +8198,16 @@
     </row>
     <row r="71" spans="1:37" ht="13" x14ac:dyDescent="0.15">
       <c r="A71" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B71" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C71" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D71" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B71" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C71" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D71" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E71" s="37"/>
       <c r="F71" s="37"/>
@@ -8255,16 +8246,16 @@
     </row>
     <row r="72" spans="1:37" ht="13" x14ac:dyDescent="0.15">
       <c r="A72" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B72" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C72" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D72" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B72" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C72" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D72" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E72" s="37"/>
       <c r="F72" s="37"/>
@@ -8303,16 +8294,16 @@
     </row>
     <row r="73" spans="1:37" ht="13" x14ac:dyDescent="0.15">
       <c r="A73" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B73" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C73" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D73" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B73" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C73" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D73" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E73" s="37"/>
       <c r="F73" s="37"/>
@@ -8351,16 +8342,16 @@
     </row>
     <row r="74" spans="1:37" ht="13" x14ac:dyDescent="0.15">
       <c r="A74" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B74" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C74" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D74" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B74" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C74" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D74" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E74" s="37"/>
       <c r="F74" s="37"/>
@@ -8399,16 +8390,16 @@
     </row>
     <row r="75" spans="1:37" ht="13" x14ac:dyDescent="0.15">
       <c r="A75" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B75" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C75" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D75" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B75" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C75" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D75" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E75" s="37"/>
       <c r="F75" s="37"/>
@@ -11398,25 +11389,25 @@
     </row>
     <row r="2" spans="1:55" ht="13" x14ac:dyDescent="0.15">
       <c r="A2" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B2" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C2" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D2" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B2" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C2" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D2" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E2" s="26">
         <v>1</v>
       </c>
       <c r="F2" s="124" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="G2" s="124" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="H2" s="124" t="s">
         <v>71</v>
@@ -11432,25 +11423,25 @@
     </row>
     <row r="3" spans="1:55" ht="13" x14ac:dyDescent="0.15">
       <c r="A3" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B3" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C3" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D3" s="124" t="s">
         <v>260</v>
       </c>
-      <c r="B3" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C3" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D3" s="124" t="s">
+      <c r="E3" s="124" t="s">
         <v>262</v>
       </c>
-      <c r="E3" s="124" t="s">
-        <v>264</v>
-      </c>
       <c r="F3" s="124" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="G3" s="124" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="H3" s="124" t="s">
         <v>71</v>
@@ -11465,25 +11456,25 @@
     </row>
     <row r="4" spans="1:55" ht="13" x14ac:dyDescent="0.15">
       <c r="A4" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B4" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C4" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D4" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B4" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C4" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D4" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E4" s="26">
         <v>2</v>
       </c>
       <c r="F4" s="124" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="G4" s="124" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="H4" s="124" t="s">
         <v>71</v>
@@ -11498,28 +11489,28 @@
     </row>
     <row r="5" spans="1:55" ht="13" x14ac:dyDescent="0.15">
       <c r="A5" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B5" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C5" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D5" s="124" t="s">
         <v>260</v>
       </c>
-      <c r="B5" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C5" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D5" s="124" t="s">
-        <v>262</v>
-      </c>
       <c r="E5" s="124" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="F5" s="124" t="s">
+        <v>269</v>
+      </c>
+      <c r="G5" s="124" t="s">
+        <v>270</v>
+      </c>
+      <c r="H5" s="124" t="s">
         <v>271</v>
-      </c>
-      <c r="G5" s="124" t="s">
-        <v>272</v>
-      </c>
-      <c r="H5" s="124" t="s">
-        <v>273</v>
       </c>
       <c r="I5" s="37">
         <v>5</v>
@@ -11531,25 +11522,25 @@
     </row>
     <row r="6" spans="1:55" ht="13" x14ac:dyDescent="0.15">
       <c r="A6" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B6" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C6" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D6" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B6" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C6" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D6" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E6" s="26">
         <v>3</v>
       </c>
       <c r="F6" s="124" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="G6" s="124" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="H6" s="124" t="s">
         <v>71</v>
@@ -11564,25 +11555,25 @@
     </row>
     <row r="7" spans="1:55" ht="13" x14ac:dyDescent="0.15">
       <c r="A7" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B7" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C7" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D7" s="124" t="s">
         <v>260</v>
       </c>
-      <c r="B7" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C7" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D7" s="124" t="s">
-        <v>262</v>
-      </c>
       <c r="E7" s="124" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F7" s="124" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="G7" s="124" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="H7" s="124" t="s">
         <v>71</v>
@@ -11597,25 +11588,25 @@
     </row>
     <row r="8" spans="1:55" ht="13" x14ac:dyDescent="0.15">
       <c r="A8" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B8" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C8" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D8" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B8" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C8" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D8" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E8" s="26">
         <v>4</v>
       </c>
       <c r="F8" s="124" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="G8" s="124" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="H8" s="124" t="s">
         <v>71</v>
@@ -11630,25 +11621,25 @@
     </row>
     <row r="9" spans="1:55" ht="13" x14ac:dyDescent="0.15">
       <c r="A9" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B9" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C9" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D9" s="124" t="s">
         <v>260</v>
       </c>
-      <c r="B9" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C9" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D9" s="124" t="s">
-        <v>262</v>
-      </c>
       <c r="E9" s="124" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="F9" s="124" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="G9" s="124" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="H9" s="124" t="s">
         <v>71</v>
@@ -11663,25 +11654,25 @@
     </row>
     <row r="10" spans="1:55" ht="13" x14ac:dyDescent="0.15">
       <c r="A10" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B10" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C10" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D10" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B10" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C10" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D10" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E10" s="26">
         <v>5</v>
       </c>
       <c r="F10" s="124" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="G10" s="124" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="H10" s="124" t="s">
         <v>71</v>
@@ -11696,25 +11687,25 @@
     </row>
     <row r="11" spans="1:55" ht="13" x14ac:dyDescent="0.15">
       <c r="A11" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B11" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C11" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D11" s="124" t="s">
         <v>260</v>
       </c>
-      <c r="B11" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C11" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D11" s="124" t="s">
-        <v>262</v>
-      </c>
       <c r="E11" s="124" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F11" s="124" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="G11" s="124" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="H11" s="124" t="s">
         <v>71</v>
@@ -11729,25 +11720,25 @@
     </row>
     <row r="12" spans="1:55" ht="13" x14ac:dyDescent="0.15">
       <c r="A12" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B12" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C12" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D12" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B12" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C12" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D12" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E12" s="26">
         <v>6</v>
       </c>
       <c r="F12" s="124" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="G12" s="124" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="H12" s="124" t="s">
         <v>71</v>
@@ -11762,25 +11753,25 @@
     </row>
     <row r="13" spans="1:55" ht="13" x14ac:dyDescent="0.15">
       <c r="A13" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B13" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C13" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D13" s="124" t="s">
         <v>260</v>
       </c>
-      <c r="B13" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C13" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D13" s="124" t="s">
-        <v>262</v>
-      </c>
       <c r="E13" s="124" t="s">
+        <v>268</v>
+      </c>
+      <c r="F13" s="124" t="s">
+        <v>269</v>
+      </c>
+      <c r="G13" s="124" t="s">
         <v>270</v>
-      </c>
-      <c r="F13" s="124" t="s">
-        <v>271</v>
-      </c>
-      <c r="G13" s="124" t="s">
-        <v>272</v>
       </c>
       <c r="H13" s="124" t="s">
         <v>71</v>
@@ -11795,25 +11786,25 @@
     </row>
     <row r="14" spans="1:55" ht="13" x14ac:dyDescent="0.15">
       <c r="A14" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B14" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C14" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D14" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B14" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C14" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D14" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E14" s="124">
         <v>7</v>
       </c>
       <c r="F14" s="124" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="G14" s="124" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="H14" s="124" t="s">
         <v>71</v>
@@ -11828,25 +11819,25 @@
     </row>
     <row r="15" spans="1:55" ht="13" x14ac:dyDescent="0.15">
       <c r="A15" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B15" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C15" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D15" s="124" t="s">
         <v>260</v>
       </c>
-      <c r="B15" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C15" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D15" s="124" t="s">
-        <v>262</v>
-      </c>
       <c r="E15" s="124" t="s">
+        <v>267</v>
+      </c>
+      <c r="F15" s="124" t="s">
         <v>269</v>
       </c>
-      <c r="F15" s="124" t="s">
-        <v>271</v>
-      </c>
       <c r="G15" s="124" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="H15" s="124" t="s">
         <v>71</v>
@@ -14903,7 +14894,7 @@
         <v>137</v>
       </c>
       <c r="O1" s="61" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="P1" s="61" t="s">
         <v>145</v>
@@ -14945,16 +14936,16 @@
     </row>
     <row r="2" spans="1:44" ht="13" x14ac:dyDescent="0.15">
       <c r="A2" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B2" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C2" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D2" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B2" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C2" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D2" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E2" s="26">
         <v>1</v>
@@ -14972,19 +14963,19 @@
     </row>
     <row r="3" spans="1:44" ht="13" x14ac:dyDescent="0.15">
       <c r="A3" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B3" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C3" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D3" s="124" t="s">
         <v>260</v>
       </c>
-      <c r="B3" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C3" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D3" s="124" t="s">
+      <c r="E3" s="124" t="s">
         <v>262</v>
-      </c>
-      <c r="E3" s="124" t="s">
-        <v>264</v>
       </c>
       <c r="F3" s="42">
         <v>54</v>
@@ -14998,16 +14989,16 @@
     </row>
     <row r="4" spans="1:44" ht="13" x14ac:dyDescent="0.15">
       <c r="A4" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B4" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C4" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D4" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B4" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C4" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D4" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E4" s="26">
         <v>2</v>
@@ -15024,19 +15015,19 @@
     </row>
     <row r="5" spans="1:44" ht="13" x14ac:dyDescent="0.15">
       <c r="A5" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B5" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C5" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D5" s="124" t="s">
         <v>260</v>
       </c>
-      <c r="B5" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C5" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D5" s="124" t="s">
-        <v>262</v>
-      </c>
       <c r="E5" s="124" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="F5" s="42">
         <v>5</v>
@@ -15065,16 +15056,16 @@
     </row>
     <row r="6" spans="1:44" ht="13" x14ac:dyDescent="0.15">
       <c r="A6" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B6" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C6" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D6" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B6" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C6" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D6" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E6" s="26">
         <v>3</v>
@@ -15106,25 +15097,25 @@
     </row>
     <row r="7" spans="1:44" ht="13" x14ac:dyDescent="0.15">
       <c r="A7" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B7" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C7" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D7" s="124" t="s">
         <v>260</v>
       </c>
-      <c r="B7" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C7" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D7" s="124" t="s">
-        <v>262</v>
-      </c>
       <c r="E7" s="124" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F7" s="42">
         <v>2</v>
       </c>
       <c r="H7" s="44" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="O7" s="42">
         <v>1</v>
@@ -15133,21 +15124,21 @@
         <v>2</v>
       </c>
       <c r="S7" s="44" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="8" spans="1:44" ht="13" x14ac:dyDescent="0.15">
       <c r="A8" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B8" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C8" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D8" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B8" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C8" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D8" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E8" s="26">
         <v>4</v>
@@ -15170,19 +15161,19 @@
     </row>
     <row r="9" spans="1:44" ht="13" x14ac:dyDescent="0.15">
       <c r="A9" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B9" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C9" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D9" s="124" t="s">
         <v>260</v>
       </c>
-      <c r="B9" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C9" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D9" s="124" t="s">
-        <v>262</v>
-      </c>
       <c r="E9" s="124" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="G9" s="42">
         <v>1</v>
@@ -15202,16 +15193,16 @@
     </row>
     <row r="10" spans="1:44" ht="13" x14ac:dyDescent="0.15">
       <c r="A10" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B10" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C10" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D10" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B10" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C10" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D10" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E10" s="26">
         <v>5</v>
@@ -15228,19 +15219,19 @@
     </row>
     <row r="11" spans="1:44" ht="13" x14ac:dyDescent="0.15">
       <c r="A11" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B11" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C11" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D11" s="124" t="s">
         <v>260</v>
       </c>
-      <c r="B11" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C11" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D11" s="124" t="s">
-        <v>262</v>
-      </c>
       <c r="E11" s="124" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F11" s="42">
         <v>1</v>
@@ -15263,16 +15254,16 @@
     </row>
     <row r="12" spans="1:44" ht="13" x14ac:dyDescent="0.15">
       <c r="A12" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B12" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C12" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D12" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B12" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C12" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D12" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E12" s="26">
         <v>6</v>
@@ -15281,7 +15272,7 @@
         <v>33</v>
       </c>
       <c r="H12" s="44" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="J12" s="42">
         <v>1</v>
@@ -15298,22 +15289,22 @@
     </row>
     <row r="13" spans="1:44" ht="13" x14ac:dyDescent="0.15">
       <c r="A13" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B13" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C13" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D13" s="124" t="s">
         <v>260</v>
       </c>
-      <c r="B13" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C13" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D13" s="124" t="s">
-        <v>262</v>
-      </c>
       <c r="E13" s="124" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="H13" s="44" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="K13" s="42">
         <v>1</v>
@@ -15321,22 +15312,22 @@
     </row>
     <row r="14" spans="1:44" ht="13" x14ac:dyDescent="0.15">
       <c r="A14" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B14" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C14" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D14" s="124" t="s">
         <v>260</v>
-      </c>
-      <c r="B14" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C14" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D14" s="124" t="s">
-        <v>262</v>
       </c>
       <c r="E14" s="124">
         <v>7</v>
       </c>
       <c r="H14" s="44" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="I14" s="42">
         <v>1</v>
@@ -15350,19 +15341,19 @@
     </row>
     <row r="15" spans="1:44" ht="13" x14ac:dyDescent="0.15">
       <c r="A15" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="B15" s="125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C15" s="125" t="s">
+        <v>259</v>
+      </c>
+      <c r="D15" s="124" t="s">
         <v>260</v>
       </c>
-      <c r="B15" s="125" t="s">
-        <v>258</v>
-      </c>
-      <c r="C15" s="125" t="s">
-        <v>261</v>
-      </c>
-      <c r="D15" s="124" t="s">
-        <v>262</v>
-      </c>
       <c r="E15" s="124" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="H15" s="44" t="s">
         <v>71</v>
@@ -18378,7 +18369,7 @@
     </row>
     <row r="2" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A2" s="65" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B2" s="34"/>
     </row>
@@ -18387,7 +18378,7 @@
     </row>
     <row r="4" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A4" s="65" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B4" s="34"/>
       <c r="C4" s="34"/>
@@ -18403,13 +18394,13 @@
         <v>61</v>
       </c>
       <c r="B6" s="123" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C6" s="56" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D6" s="126" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -19076,8 +19067,8 @@
   </sheetPr>
   <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -19088,23 +19079,17 @@
   <sheetData>
     <row r="1" spans="1:1" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="15" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="18" t="s">
-        <v>150</v>
-      </c>
+      <c r="A2" s="18"/>
     </row>
     <row r="3" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="18" t="s">
-        <v>148</v>
-      </c>
+      <c r="A3" s="18"/>
     </row>
     <row r="7" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="18" t="s">
-        <v>281</v>
-      </c>
+      <c r="A7" s="18"/>
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="Kib2gtiduhw5EERTZ4siKToKaKfdxhLCdbzrtoxKlqyxyF5FnEhw3OfFZF11vVNYtP5a9Ctc1H8F+L8m6CZbzw==" saltValue="kE6sMLi4pxInD7azmDrhDA==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertRows="0" insertHyperlinks="0" sort="0" autoFilter="0"/>

</xml_diff>

<commit_message>
Added more flaws to the test dataset to see if the app catches them
</commit_message>
<xml_diff>
--- a/Test Data/Nick HV Fake Data.xlsx
+++ b/Test Data/Nick HV Fake Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nick.lyon/Documents/Jobs/2021_HerbVar Network Admin/HerbVar-Data-Portal/Test Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58184B2F-3864-BB4D-BFBD-4EAB92739E71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{479ECDAD-4AE7-CD41-9979-7CE13CA87907}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-51160" yWindow="2780" windowWidth="21340" windowHeight="21140" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-51160" yWindow="2780" windowWidth="21340" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="siteData" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="819" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="287">
   <si>
     <t>variable</t>
   </si>
@@ -1274,12 +1274,6 @@
     <t>many thrips</t>
   </si>
   <si>
-    <t>words</t>
-  </si>
-  <si>
-    <t>Wanted to try out adding columns to the siteData tab</t>
-  </si>
-  <si>
     <t>1q</t>
   </si>
   <si>
@@ -1308,6 +1302,18 @@
   </si>
   <si>
     <t>October 14th, 2021</t>
+  </si>
+  <si>
+    <t>October</t>
+  </si>
+  <si>
+    <t>the 14th</t>
+  </si>
+  <si>
+    <t>bonusReproColumn</t>
+  </si>
+  <si>
+    <t>primary</t>
   </si>
 </sst>
 </file>
@@ -2185,9 +2191,9 @@
   </sheetPr>
   <dimension ref="A1:BZ23"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
+      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2339,7 +2345,9 @@
       <c r="A6" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="B6" s="2"/>
+      <c r="B6" s="2">
+        <v>91.051959999999994</v>
+      </c>
       <c r="C6" s="1" t="s">
         <v>4</v>
       </c>
@@ -2411,7 +2419,9 @@
       <c r="A11" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="B11" s="122"/>
+      <c r="B11" s="122" t="s">
+        <v>286</v>
+      </c>
       <c r="C11" s="3" t="s">
         <v>234</v>
       </c>
@@ -2592,7 +2602,7 @@
   <dimension ref="A1:AT101"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
@@ -4209,7 +4219,7 @@
       <c r="AA90" s="61"/>
       <c r="AB90" s="61"/>
     </row>
-    <row r="91" spans="1:28" ht="14" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:28" ht="28" x14ac:dyDescent="0.15">
       <c r="A91" s="80" t="s">
         <v>214</v>
       </c>
@@ -4455,7 +4465,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="126" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E7" s="18" t="s">
         <v>254</v>
@@ -4485,7 +4495,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E10" s="9"/>
     </row>
@@ -4522,9 +4532,9 @@
   </sheetPr>
   <dimension ref="A1:BJ1000"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="AR1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J10" sqref="J10"/>
+      <selection pane="bottomLeft" activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4720,7 +4730,7 @@
         <v>164</v>
       </c>
       <c r="BB1" s="30" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="BC1" s="29"/>
       <c r="BD1" s="29"/>
@@ -4779,7 +4789,7 @@
         <v>5</v>
       </c>
       <c r="Q2" s="39" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="R2" s="38">
         <v>5</v>
@@ -4792,7 +4802,7 @@
         <v>269</v>
       </c>
       <c r="V2" s="41" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="W2" s="37">
         <v>5</v>
@@ -4934,7 +4944,7 @@
         <v>5</v>
       </c>
       <c r="Q3" s="39" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="R3" s="38">
         <v>45</v>
@@ -4947,7 +4957,7 @@
         <v>270</v>
       </c>
       <c r="V3" s="41" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="W3" s="37">
         <v>5</v>
@@ -5081,7 +5091,7 @@
         <v>5</v>
       </c>
       <c r="Q4" s="39" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="R4" s="38">
         <v>5</v>
@@ -5094,7 +5104,7 @@
         <v>270</v>
       </c>
       <c r="V4" s="41" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="W4" s="37">
         <v>5</v>
@@ -5228,7 +5238,7 @@
         <v>5</v>
       </c>
       <c r="Q5" s="39" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="R5" s="38">
         <v>5</v>
@@ -5241,7 +5251,7 @@
         <v>271</v>
       </c>
       <c r="V5" s="41" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="W5" s="37">
         <v>5</v>
@@ -5371,7 +5381,7 @@
       </c>
       <c r="P6" s="38"/>
       <c r="Q6" s="39" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="R6" s="38">
         <v>3</v>
@@ -5384,7 +5394,7 @@
         <v>271</v>
       </c>
       <c r="V6" s="41" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="W6" s="37">
         <v>5</v>
@@ -5514,7 +5524,7 @@
       </c>
       <c r="P7" s="38"/>
       <c r="Q7" s="39" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="R7" s="38">
         <v>1</v>
@@ -5527,7 +5537,7 @@
         <v>271</v>
       </c>
       <c r="V7" s="41" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="W7" s="37"/>
       <c r="X7" s="37"/>
@@ -5583,7 +5593,7 @@
         <v>5</v>
       </c>
       <c r="Q8" s="39" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="R8" s="38">
         <v>1</v>
@@ -5596,7 +5606,7 @@
         <v>271</v>
       </c>
       <c r="V8" s="41" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="W8" s="37">
         <v>5</v>
@@ -5694,7 +5704,7 @@
       <c r="A9" s="123"/>
       <c r="B9" s="124"/>
       <c r="C9" s="124" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D9" s="123"/>
       <c r="E9" s="37">
@@ -5730,7 +5740,7 @@
         <v>5</v>
       </c>
       <c r="Q9" s="39" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="R9" s="38">
         <v>1</v>
@@ -5743,7 +5753,7 @@
         <v>271</v>
       </c>
       <c r="V9" s="41" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="W9" s="37">
         <v>5</v>
@@ -5841,7 +5851,7 @@
       <c r="A10" s="123"/>
       <c r="B10" s="124"/>
       <c r="C10" s="124" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D10" s="123"/>
       <c r="E10" s="37">
@@ -5877,7 +5887,7 @@
         <v>5</v>
       </c>
       <c r="Q10" s="39" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="R10" s="38">
         <v>1</v>
@@ -5890,7 +5900,7 @@
         <v>271</v>
       </c>
       <c r="V10" s="41" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="W10" s="37">
         <v>5</v>
@@ -6026,7 +6036,7 @@
         <v>5</v>
       </c>
       <c r="Q11" s="39" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="R11" s="38">
         <v>30</v>
@@ -6039,7 +6049,7 @@
         <v>271</v>
       </c>
       <c r="V11" s="41" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="W11" s="37">
         <v>5</v>
@@ -6173,7 +6183,7 @@
         <v>5</v>
       </c>
       <c r="Q12" s="39" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="R12" s="38">
         <v>5</v>
@@ -6186,7 +6196,7 @@
         <v>271</v>
       </c>
       <c r="V12" s="41" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="W12" s="37">
         <v>5</v>
@@ -6320,7 +6330,7 @@
         <v>5</v>
       </c>
       <c r="Q13" s="39" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="R13" s="38"/>
       <c r="S13" s="37"/>
@@ -6331,7 +6341,7 @@
         <v>271</v>
       </c>
       <c r="V13" s="41" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="W13" s="37">
         <v>5</v>
@@ -6443,13 +6453,13 @@
         <v>80</v>
       </c>
       <c r="I14" s="37" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="J14" s="37" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="K14" s="37" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="L14" s="37"/>
       <c r="M14" s="27" t="s">
@@ -6465,7 +6475,7 @@
         <v>5</v>
       </c>
       <c r="Q14" s="39" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="R14" s="38"/>
       <c r="S14" s="37"/>
@@ -6476,7 +6486,7 @@
         <v>271</v>
       </c>
       <c r="V14" s="41" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="W14" s="37">
         <v>5</v>
@@ -6610,7 +6620,7 @@
         <v>5</v>
       </c>
       <c r="Q15" s="39" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="R15" s="38"/>
       <c r="S15" s="37"/>
@@ -6621,7 +6631,7 @@
         <v>271</v>
       </c>
       <c r="V15" s="41" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="W15" s="37">
         <v>5</v>
@@ -11667,9 +11677,9 @@
   </sheetPr>
   <dimension ref="A1:BC1000"/>
   <sheetViews>
-    <sheetView topLeftCell="AF1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="AD1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G41" sqref="G41"/>
+      <selection pane="bottomLeft" activeCell="AK21" sqref="AK21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -11805,7 +11815,9 @@
       <c r="AI1" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="AJ1" s="23"/>
+      <c r="AJ1" s="23" t="s">
+        <v>285</v>
+      </c>
       <c r="AK1" s="23"/>
       <c r="AL1" s="23"/>
       <c r="AM1" s="23"/>
@@ -11960,18 +11972,10 @@
       <c r="AD5" s="37"/>
     </row>
     <row r="6" spans="1:55" ht="13" x14ac:dyDescent="0.15">
-      <c r="A6" s="123" t="s">
-        <v>255</v>
-      </c>
-      <c r="B6" s="124" t="s">
-        <v>253</v>
-      </c>
-      <c r="C6" s="124" t="s">
-        <v>256</v>
-      </c>
-      <c r="D6" s="123" t="s">
-        <v>257</v>
-      </c>
+      <c r="A6" s="123"/>
+      <c r="B6" s="124"/>
+      <c r="C6" s="124"/>
+      <c r="D6" s="123"/>
       <c r="E6" s="26">
         <v>3</v>
       </c>
@@ -12021,7 +12025,7 @@
         <v>8</v>
       </c>
       <c r="J7" s="37">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AD7" s="37"/>
     </row>
@@ -12032,8 +12036,8 @@
       <c r="B8" s="124" t="s">
         <v>253</v>
       </c>
-      <c r="C8" s="124" t="s">
-        <v>256</v>
+      <c r="C8" s="124">
+        <v>44483</v>
       </c>
       <c r="D8" s="123" t="s">
         <v>257</v>
@@ -12086,9 +12090,6 @@
       <c r="I9" s="37">
         <v>3</v>
       </c>
-      <c r="J9" s="37">
-        <v>5</v>
-      </c>
       <c r="AD9" s="37"/>
     </row>
     <row r="10" spans="1:55" ht="13" x14ac:dyDescent="0.15">
@@ -12125,15 +12126,9 @@
       <c r="AD10" s="37"/>
     </row>
     <row r="11" spans="1:55" ht="13" x14ac:dyDescent="0.15">
-      <c r="A11" s="123" t="s">
-        <v>255</v>
-      </c>
-      <c r="B11" s="124" t="s">
-        <v>253</v>
-      </c>
-      <c r="C11" s="124" t="s">
-        <v>256</v>
-      </c>
+      <c r="A11" s="123"/>
+      <c r="B11" s="124"/>
+      <c r="C11" s="124"/>
       <c r="D11" s="123" t="s">
         <v>257</v>
       </c>
@@ -12148,9 +12143,6 @@
       </c>
       <c r="H11" s="123" t="s">
         <v>71</v>
-      </c>
-      <c r="I11" s="37">
-        <v>4</v>
       </c>
       <c r="J11" s="37">
         <v>2</v>
@@ -12252,7 +12244,7 @@
         <v>9</v>
       </c>
       <c r="J14" s="37">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="AD14" s="37"/>
     </row>
@@ -15262,9 +15254,9 @@
   </sheetPr>
   <dimension ref="A1:AR1000"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="P1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U2" sqref="U2"/>
+      <selection pane="bottomLeft" activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -15348,10 +15340,10 @@
         <v>3</v>
       </c>
       <c r="T1" s="31" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="U1" s="31" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="V1" s="31"/>
       <c r="W1" s="31"/>
@@ -15426,9 +15418,7 @@
       <c r="G3" s="41">
         <v>8</v>
       </c>
-      <c r="H3" s="43" t="s">
-        <v>71</v>
-      </c>
+      <c r="H3" s="43"/>
     </row>
     <row r="4" spans="1:44" ht="13" x14ac:dyDescent="0.15">
       <c r="A4" s="123" t="s">
@@ -15475,9 +15465,7 @@
       <c r="F5" s="41">
         <v>5</v>
       </c>
-      <c r="H5" s="43" t="s">
-        <v>71</v>
-      </c>
+      <c r="H5" s="43"/>
       <c r="I5" s="41">
         <v>8</v>
       </c>
@@ -15603,18 +15591,10 @@
       </c>
     </row>
     <row r="9" spans="1:44" ht="13" x14ac:dyDescent="0.15">
-      <c r="A9" s="123" t="s">
-        <v>255</v>
-      </c>
-      <c r="B9" s="124" t="s">
-        <v>253</v>
-      </c>
-      <c r="C9" s="124" t="s">
-        <v>256</v>
-      </c>
-      <c r="D9" s="123" t="s">
-        <v>257</v>
-      </c>
+      <c r="A9" s="123"/>
+      <c r="B9" s="124"/>
+      <c r="C9" s="124"/>
+      <c r="D9" s="123"/>
       <c r="E9" s="123" t="s">
         <v>261</v>
       </c>
@@ -15635,18 +15615,10 @@
       </c>
     </row>
     <row r="10" spans="1:44" ht="13" x14ac:dyDescent="0.15">
-      <c r="A10" s="123" t="s">
-        <v>255</v>
-      </c>
-      <c r="B10" s="124" t="s">
-        <v>253</v>
-      </c>
-      <c r="C10" s="124" t="s">
-        <v>256</v>
-      </c>
-      <c r="D10" s="123" t="s">
-        <v>257</v>
-      </c>
+      <c r="A10" s="123"/>
+      <c r="B10" s="124"/>
+      <c r="C10" s="124"/>
+      <c r="D10" s="123"/>
       <c r="E10" s="26">
         <v>5</v>
       </c>
@@ -15738,7 +15710,7 @@
         <v>253</v>
       </c>
       <c r="C13" s="124" t="s">
-        <v>256</v>
+        <v>283</v>
       </c>
       <c r="D13" s="123" t="s">
         <v>257</v>
@@ -15761,7 +15733,7 @@
         <v>253</v>
       </c>
       <c r="C14" s="124" t="s">
-        <v>256</v>
+        <v>284</v>
       </c>
       <c r="D14" s="123" t="s">
         <v>257</v>
@@ -18784,7 +18756,7 @@
   <sheetViews>
     <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
+      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -18810,19 +18782,11 @@
         <v>116</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="14" x14ac:dyDescent="0.15">
-      <c r="A2" s="64" t="s">
-        <v>61</v>
-      </c>
-      <c r="B2" s="122" t="s">
-        <v>250</v>
-      </c>
-      <c r="C2" s="55" t="s">
-        <v>273</v>
-      </c>
-      <c r="D2" s="125" t="s">
-        <v>274</v>
-      </c>
+    <row r="2" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+      <c r="A2" s="64"/>
+      <c r="B2" s="122"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="125"/>
     </row>
     <row r="3" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="B3" s="34"/>
@@ -19488,7 +19452,7 @@
   </sheetPr>
   <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>

</xml_diff>